<commit_message>
[Add metric and dispertion]
</commit_message>
<xml_diff>
--- a/current_field.xlsx
+++ b/current_field.xlsx
@@ -588,7 +588,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>r</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -620,7 +620,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>g</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>g</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -697,12 +697,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>r</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>r</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -739,7 +739,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>g</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>g</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -930,12 +930,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>r</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>res</t>
+          <t>g</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -945,12 +945,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>g</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>res</t>
+          <t>g</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1007,17 +1007,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>i</t>
+          <t>r</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>g</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>r</t>
+          <t>g</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">

</xml_diff>